<commit_message>
MapPrototype3 - Minor edit
Minor edits to map
</commit_message>
<xml_diff>
--- a/Assets/MapPrototypeDesign.xlsx
+++ b/Assets/MapPrototypeDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TL\Personal\Projects_Self\2023gamejamcssa\2023gamejamcssa\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9909C714-B4E7-4264-910A-1F4AF85C36F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385024B3-AC53-4047-AF8D-ED4920013FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{F6FA76B0-B0FB-44AE-A37A-4F9737DD96F1}"/>
+    <workbookView xWindow="15888" yWindow="6084" windowWidth="7500" windowHeight="6000" activeTab="2" xr2:uid="{F6FA76B0-B0FB-44AE-A37A-4F9737DD96F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1007,7 +1007,7 @@
   <dimension ref="A1:AW32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="46" zoomScaleNormal="46" workbookViewId="0">
-      <selection activeCell="AD24" sqref="AD24"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1771,8 +1771,8 @@
       <c r="B9" s="4">
         <v>0</v>
       </c>
-      <c r="C9" s="4">
-        <v>0</v>
+      <c r="C9" s="56">
+        <v>11</v>
       </c>
       <c r="D9" s="64">
         <v>4</v>
@@ -1863,8 +1863,8 @@
       <c r="B10" s="4">
         <v>0</v>
       </c>
-      <c r="C10" s="4">
-        <v>0</v>
+      <c r="C10" s="56">
+        <v>11</v>
       </c>
       <c r="D10" s="4">
         <v>0</v>
@@ -2431,11 +2431,11 @@
       <c r="B16" s="4">
         <v>0</v>
       </c>
-      <c r="C16" s="4">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
+      <c r="C16" s="56">
+        <v>11</v>
+      </c>
+      <c r="D16" s="56">
+        <v>11</v>
       </c>
       <c r="E16" s="56">
         <v>11</v>
@@ -2526,11 +2526,11 @@
       <c r="B17" s="4">
         <v>0</v>
       </c>
-      <c r="C17" s="4">
-        <v>0</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0</v>
+      <c r="C17" s="56">
+        <v>11</v>
+      </c>
+      <c r="D17" s="56">
+        <v>11</v>
       </c>
       <c r="E17" s="56">
         <v>11</v>
@@ -3915,7 +3915,7 @@
   <dimension ref="B1:AW31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="46" zoomScaleNormal="46" workbookViewId="0">
-      <selection activeCell="AD24" sqref="AD24"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4274,7 +4274,9 @@
     </row>
     <row r="9" spans="2:42" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="2"/>
-      <c r="C9" s="4"/>
+      <c r="C9" s="55">
+        <v>11</v>
+      </c>
       <c r="D9" s="65">
         <v>4</v>
       </c>
@@ -4329,7 +4331,9 @@
     </row>
     <row r="10" spans="2:42" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
+      <c r="C10" s="55">
+        <v>11</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="4"/>
       <c r="F10" s="2"/>
@@ -4643,8 +4647,12 @@
     </row>
     <row r="16" spans="2:42" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="C16" s="55">
+        <v>11</v>
+      </c>
+      <c r="D16" s="55">
+        <v>11</v>
+      </c>
       <c r="E16" s="55">
         <v>11</v>
       </c>
@@ -4692,8 +4700,12 @@
     </row>
     <row r="17" spans="2:35" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="C17" s="55">
+        <v>11</v>
+      </c>
+      <c r="D17" s="55">
+        <v>11</v>
+      </c>
       <c r="E17" s="55">
         <v>11</v>
       </c>
@@ -5286,7 +5298,7 @@
   <dimension ref="A1:AW32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="46" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="AD24" sqref="AD24"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6103,8 +6115,8 @@
       <c r="B9" s="4">
         <v>0</v>
       </c>
-      <c r="C9" s="4">
-        <v>0</v>
+      <c r="C9" s="55">
+        <v>11</v>
       </c>
       <c r="D9" s="64">
         <v>4</v>
@@ -6201,8 +6213,8 @@
       <c r="B10" s="4">
         <v>0</v>
       </c>
-      <c r="C10" s="4">
-        <v>0</v>
+      <c r="C10" s="55">
+        <v>11</v>
       </c>
       <c r="D10" s="4">
         <v>0</v>
@@ -6798,11 +6810,11 @@
       <c r="B16" s="4">
         <v>0</v>
       </c>
-      <c r="C16" s="4">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
+      <c r="C16" s="55">
+        <v>11</v>
+      </c>
+      <c r="D16" s="55">
+        <v>11</v>
       </c>
       <c r="E16" s="55">
         <v>11</v>
@@ -6896,11 +6908,11 @@
       <c r="B17" s="4">
         <v>0</v>
       </c>
-      <c r="C17" s="4">
-        <v>0</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0</v>
+      <c r="C17" s="55">
+        <v>11</v>
+      </c>
+      <c r="D17" s="55">
+        <v>11</v>
       </c>
       <c r="E17" s="55">
         <v>11</v>

</xml_diff>